<commit_message>
updated figures, large paper update on feedback study
</commit_message>
<xml_diff>
--- a/visualizations.xlsx
+++ b/visualizations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2160" windowHeight="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2160" windowHeight="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="p2" sheetId="1" r:id="rId1"/>
@@ -57,9 +57,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -122,7 +123,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -179,175 +179,175 @@
             <c:numRef>
               <c:f>'p2'!$B$1:$B$56</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="56"/>
                 <c:pt idx="0">
-                  <c:v>41810</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41811</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41812</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41813</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41814</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>41815</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>41816</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41817</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>41818</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>41819</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>41826</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>41827</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>41828</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>41829</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>41830</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>41831</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>41832</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>41833</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>41834</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>41835</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>41836</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>41837</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>41838</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>41839</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>41840</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>41841</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>41842</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>41843</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>41844</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>41845</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>41846</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>41847</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>41848</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>41849</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>41850</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>41851</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>41852</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>41853</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>41854</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>41855</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>41856</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>41857</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>41858</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>41859</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>41860</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>41861</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>41862</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>41863</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>41864</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>41865</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>41866</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>41867</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>41868</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>41869</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>41870</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>41871</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -540,8 +540,8 @@
         </c:dLbls>
         <c:gapWidth val="10"/>
         <c:overlap val="-27"/>
-        <c:axId val="845878192"/>
-        <c:axId val="845871120"/>
+        <c:axId val="2058063840"/>
+        <c:axId val="2058064928"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -568,175 +568,175 @@
             <c:numRef>
               <c:f>'p2'!$B$1:$B$56</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="56"/>
                 <c:pt idx="0">
-                  <c:v>41810</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41811</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41812</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41813</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41814</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>41815</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>41816</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41817</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>41818</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>41819</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>41826</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>41827</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>41828</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>41829</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>41830</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>41831</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>41832</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>41833</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>41834</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>41835</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>41836</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>41837</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>41838</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>41839</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>41840</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>41841</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>41842</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>41843</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>41844</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>41845</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>41846</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>41847</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>41848</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>41849</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>41850</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>41851</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>41852</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>41853</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>41854</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>41855</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>41856</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>41857</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>41858</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>41859</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>41860</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>41861</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>41862</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>41863</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>41864</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>41865</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>41866</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>41867</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>41868</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>41869</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>41870</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>41871</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -930,17 +930,17 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="845879824"/>
-        <c:axId val="845879280"/>
+        <c:axId val="2058070368"/>
+        <c:axId val="2058062208"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="845878192"/>
+        <c:axId val="2058063840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -977,14 +977,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="845871120"/>
+        <c:crossAx val="2058064928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="845871120"/>
+        <c:axId val="2058064928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1035,12 +1035,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="845878192"/>
+        <c:crossAx val="2058063840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="845879280"/>
+        <c:axId val="2058062208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1079,26 +1079,28 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="845879824"/>
+        <c:crossAx val="2058070368"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
-      <c:dateAx>
-        <c:axId val="845879824"/>
+      <c:catAx>
+        <c:axId val="2058070368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="845879280"/>
+        <c:crossAx val="2058062208"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1109,7 +1111,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1216,7 +1217,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1273,175 +1273,175 @@
             <c:numRef>
               <c:f>'p3'!$B$1:$B$56</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="56"/>
                 <c:pt idx="0">
-                  <c:v>41810</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41811</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41812</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41813</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41814</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>41815</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>41816</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41817</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>41818</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>41819</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>41833</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>41834</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>41835</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>41836</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>41837</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>41838</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>41839</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>41840</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>41841</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>41842</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>41843</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>41844</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>41845</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>41846</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>41847</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>41848</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>41849</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>41850</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>41851</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>41852</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>41853</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>41854</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>41855</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>41856</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>41857</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>41858</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>41859</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>41860</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>41861</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>41862</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>41863</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>41864</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>41865</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>41866</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>41867</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>41868</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>41869</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>41870</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>41871</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>41872</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>41873</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>41874</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>41875</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>41876</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>41877</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>41878</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1634,8 +1634,8 @@
         </c:dLbls>
         <c:gapWidth val="10"/>
         <c:overlap val="-27"/>
-        <c:axId val="826012368"/>
-        <c:axId val="826016720"/>
+        <c:axId val="2058068736"/>
+        <c:axId val="2058069280"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1662,175 +1662,175 @@
             <c:numRef>
               <c:f>'p3'!$B$1:$B$56</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="56"/>
                 <c:pt idx="0">
-                  <c:v>41810</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41811</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41812</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41813</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41814</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>41815</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>41816</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41817</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>41818</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>41819</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>41833</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>41834</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>41835</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>41836</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>41837</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>41838</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>41839</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>41840</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>41841</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>41842</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>41843</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>41844</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>41845</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>41846</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>41847</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>41848</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>41849</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>41850</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>41851</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>41852</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>41853</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>41854</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>41855</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>41856</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>41857</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>41858</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>41859</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>41860</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>41861</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>41862</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>41863</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>41864</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>41865</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>41866</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>41867</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>41868</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>41869</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>41870</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>41871</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>41872</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>41873</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>41874</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>41875</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>41876</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>41877</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>41878</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2024,17 +2024,17 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="828414672"/>
-        <c:axId val="828413584"/>
+        <c:axId val="2058069824"/>
+        <c:axId val="2058066016"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="826012368"/>
+        <c:axId val="2058068736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2071,7 +2071,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="826016720"/>
+        <c:crossAx val="2058069280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
@@ -2080,7 +2080,7 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="826016720"/>
+        <c:axId val="2058069280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2131,12 +2131,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="826012368"/>
+        <c:crossAx val="2058068736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="828413584"/>
+        <c:axId val="2058066016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="60"/>
@@ -2174,26 +2174,28 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="828414672"/>
+        <c:crossAx val="2058069824"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
-      <c:dateAx>
-        <c:axId val="828414672"/>
+      <c:catAx>
+        <c:axId val="2058069824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="828413584"/>
+        <c:crossAx val="2058066016"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2204,7 +2206,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2368,175 +2369,175 @@
             <c:numRef>
               <c:f>'p5'!$B$1:$B$56</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="56"/>
                 <c:pt idx="0">
-                  <c:v>41811</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41812</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41813</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41814</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41815</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>41816</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>41817</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41818</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>41819</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>41820</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>41821</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>41822</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>41823</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>41824</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>41825</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>41826</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>41827</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>41828</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>41829</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>41830</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>41831</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>41832</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>41833</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>41834</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>41835</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>41836</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>41837</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>41838</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>41839</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>41840</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>41841</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>41842</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>41843</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>41844</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>41845</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>41846</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>41847</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>41848</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>41849</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>41850</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>41851</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>41852</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>41853</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>41854</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>41855</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>41856</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>41857</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>41858</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>41859</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>41860</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>41861</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>41862</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>41863</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>41864</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>41865</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>41866</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2729,8 +2730,8 @@
         </c:dLbls>
         <c:gapWidth val="10"/>
         <c:overlap val="-27"/>
-        <c:axId val="845877648"/>
-        <c:axId val="845874928"/>
+        <c:axId val="2058074720"/>
+        <c:axId val="2058064384"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2757,175 +2758,175 @@
             <c:numRef>
               <c:f>'p5'!$B$1:$B$56</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="56"/>
                 <c:pt idx="0">
-                  <c:v>41811</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41812</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41813</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41814</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41815</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>41816</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>41817</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41818</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>41819</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>41820</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>41821</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>41822</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>41823</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>41824</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>41825</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>41826</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>41827</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>41828</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>41829</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>41830</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>41831</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>41832</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>41833</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>41834</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>41835</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>41836</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>41837</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>41838</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>41839</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>41840</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>41841</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>41842</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>41843</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>41844</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>41845</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>41846</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>41847</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>41848</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>41849</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>41850</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>41851</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>41852</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>41853</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>41854</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>41855</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>41856</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>41857</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>41858</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>41859</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>41860</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>41861</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>41862</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>41863</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>41864</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>41865</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>41866</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3119,17 +3120,17 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="846694208"/>
-        <c:axId val="846687680"/>
+        <c:axId val="2058063296"/>
+        <c:axId val="2058070912"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="845877648"/>
+        <c:axId val="2058074720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3166,7 +3167,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="845874928"/>
+        <c:crossAx val="2058064384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
@@ -3175,7 +3176,7 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="845874928"/>
+        <c:axId val="2058064384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3226,12 +3227,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="845877648"/>
+        <c:crossAx val="2058074720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="846687680"/>
+        <c:axId val="2058070912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="60"/>
@@ -3269,26 +3270,28 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="846694208"/>
+        <c:crossAx val="2058063296"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
-      <c:dateAx>
-        <c:axId val="846694208"/>
+      <c:catAx>
+        <c:axId val="2058063296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="846687680"/>
+        <c:crossAx val="2058070912"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -3463,175 +3466,175 @@
             <c:numRef>
               <c:f>'p7'!$B$1:$B$56</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="56"/>
                 <c:pt idx="0">
-                  <c:v>41829</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41830</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41831</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41832</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41833</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>41834</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>41835</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41836</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>41837</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>41838</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>41839</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>41840</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>41841</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>41842</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>41843</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>41844</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>41845</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>41846</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>41847</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>41848</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>41849</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>41850</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>41851</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>41852</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>41853</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>41854</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>41855</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>41856</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>41857</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>41858</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>41859</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>41860</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>41861</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>41862</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>41863</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>41864</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>41865</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>41866</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>41867</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>41868</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>41869</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>41870</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>41871</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>41872</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>41873</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>41874</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>41875</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>41876</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>41877</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>41878</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>41879</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>41880</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>41881</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>41882</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>41883</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>41884</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3824,8 +3827,8 @@
         </c:dLbls>
         <c:gapWidth val="11"/>
         <c:overlap val="-27"/>
-        <c:axId val="819143760"/>
-        <c:axId val="819145392"/>
+        <c:axId val="2058072000"/>
+        <c:axId val="2058061664"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -3852,175 +3855,175 @@
             <c:numRef>
               <c:f>'p7'!$B$1:$B$56</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="56"/>
                 <c:pt idx="0">
-                  <c:v>41829</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41830</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41831</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41832</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41833</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>41834</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>41835</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41836</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>41837</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>41838</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>41839</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>41840</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>41841</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>41842</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>41843</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>41844</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>41845</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>41846</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>41847</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>41848</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>41849</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>41850</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>41851</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>41852</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>41853</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>41854</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>41855</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>41856</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>41857</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>41858</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>41859</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>41860</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>41861</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>41862</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>41863</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>41864</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>41865</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>41866</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>41867</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>41868</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>41869</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>41870</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>41871</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>41872</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>41873</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>41874</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>41875</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>41876</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>41877</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>41878</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>41879</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>41880</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>41881</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>41882</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>41883</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>41884</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4214,17 +4217,17 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="828409776"/>
-        <c:axId val="828411952"/>
+        <c:axId val="2058073632"/>
+        <c:axId val="2058072544"/>
       </c:lineChart>
-      <c:dateAx>
-        <c:axId val="819143760"/>
+      <c:catAx>
+        <c:axId val="2058072000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4261,14 +4264,15 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="819145392"/>
+        <c:crossAx val="2058061664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
-        <c:axId val="819145392"/>
+        <c:axId val="2058061664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4319,12 +4323,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="819143760"/>
+        <c:crossAx val="2058072000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="828411952"/>
+        <c:axId val="2058072544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="60"/>
@@ -4362,26 +4366,28 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="828409776"/>
+        <c:crossAx val="2058073632"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
-      <c:dateAx>
-        <c:axId val="828409776"/>
+      <c:catAx>
+        <c:axId val="2058073632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="828411952"/>
+        <c:crossAx val="2058072544"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -7036,13 +7042,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7050,8 +7056,8 @@
       <c r="A1" t="b">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
-        <v>41810</v>
+      <c r="B1" s="2">
+        <v>1</v>
       </c>
       <c r="C1">
         <v>0</v>
@@ -7082,8 +7088,8 @@
       <c r="A2" t="b">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
-        <v>41811</v>
+      <c r="B2" s="2">
+        <v>2</v>
       </c>
       <c r="C2">
         <v>25.366666670000001</v>
@@ -7114,8 +7120,8 @@
       <c r="A3" t="b">
         <v>0</v>
       </c>
-      <c r="B3" s="1">
-        <v>41812</v>
+      <c r="B3" s="2">
+        <v>3</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -7146,8 +7152,8 @@
       <c r="A4" t="b">
         <v>0</v>
       </c>
-      <c r="B4" s="1">
-        <v>41813</v>
+      <c r="B4" s="2">
+        <v>4</v>
       </c>
       <c r="C4">
         <v>40.35</v>
@@ -7178,8 +7184,8 @@
       <c r="A5" t="b">
         <v>0</v>
       </c>
-      <c r="B5" s="1">
-        <v>41814</v>
+      <c r="B5" s="2">
+        <v>5</v>
       </c>
       <c r="C5">
         <v>27</v>
@@ -7210,8 +7216,8 @@
       <c r="A6" t="b">
         <v>0</v>
       </c>
-      <c r="B6" s="1">
-        <v>41815</v>
+      <c r="B6" s="2">
+        <v>6</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -7242,8 +7248,8 @@
       <c r="A7" t="b">
         <v>0</v>
       </c>
-      <c r="B7" s="1">
-        <v>41816</v>
+      <c r="B7" s="2">
+        <v>7</v>
       </c>
       <c r="C7">
         <v>67.533333330000005</v>
@@ -7274,8 +7280,8 @@
       <c r="A8" t="b">
         <v>0</v>
       </c>
-      <c r="B8" s="1">
-        <v>41817</v>
+      <c r="B8" s="2">
+        <v>8</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -7306,8 +7312,8 @@
       <c r="A9" t="b">
         <v>1</v>
       </c>
-      <c r="B9" s="1">
-        <v>41818</v>
+      <c r="B9" s="2">
+        <v>9</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -7338,8 +7344,8 @@
       <c r="A10" t="b">
         <v>1</v>
       </c>
-      <c r="B10" s="1">
-        <v>41819</v>
+      <c r="B10" s="2">
+        <v>10</v>
       </c>
       <c r="C10">
         <v>40.1</v>
@@ -7370,8 +7376,8 @@
       <c r="A11" t="b">
         <v>1</v>
       </c>
-      <c r="B11" s="1">
-        <v>41826</v>
+      <c r="B11" s="2">
+        <v>11</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -7402,8 +7408,8 @@
       <c r="A12" t="b">
         <v>1</v>
       </c>
-      <c r="B12" s="1">
-        <v>41827</v>
+      <c r="B12" s="2">
+        <v>12</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -7434,8 +7440,8 @@
       <c r="A13" t="b">
         <v>1</v>
       </c>
-      <c r="B13" s="1">
-        <v>41828</v>
+      <c r="B13" s="2">
+        <v>13</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -7466,8 +7472,8 @@
       <c r="A14" t="b">
         <v>1</v>
       </c>
-      <c r="B14" s="1">
-        <v>41829</v>
+      <c r="B14" s="2">
+        <v>14</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -7498,8 +7504,8 @@
       <c r="A15" t="b">
         <v>1</v>
       </c>
-      <c r="B15" s="1">
-        <v>41830</v>
+      <c r="B15" s="2">
+        <v>15</v>
       </c>
       <c r="C15">
         <v>26.166666670000001</v>
@@ -7530,8 +7536,8 @@
       <c r="A16" t="b">
         <v>1</v>
       </c>
-      <c r="B16" s="1">
-        <v>41831</v>
+      <c r="B16" s="2">
+        <v>16</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -7562,8 +7568,8 @@
       <c r="A17" t="b">
         <v>1</v>
       </c>
-      <c r="B17" s="1">
-        <v>41832</v>
+      <c r="B17" s="2">
+        <v>17</v>
       </c>
       <c r="C17">
         <v>80.933333329999996</v>
@@ -7594,8 +7600,8 @@
       <c r="A18" t="b">
         <v>1</v>
       </c>
-      <c r="B18" s="1">
-        <v>41833</v>
+      <c r="B18" s="2">
+        <v>18</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -7617,8 +7623,8 @@
       <c r="A19" t="b">
         <v>1</v>
       </c>
-      <c r="B19" s="1">
-        <v>41834</v>
+      <c r="B19" s="2">
+        <v>19</v>
       </c>
       <c r="C19">
         <v>40.866666670000001</v>
@@ -7640,8 +7646,8 @@
       <c r="A20" t="b">
         <v>1</v>
       </c>
-      <c r="B20" s="1">
-        <v>41835</v>
+      <c r="B20" s="2">
+        <v>20</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -7663,8 +7669,8 @@
       <c r="A21" t="b">
         <v>1</v>
       </c>
-      <c r="B21" s="1">
-        <v>41836</v>
+      <c r="B21" s="2">
+        <v>21</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -7686,8 +7692,8 @@
       <c r="A22" t="b">
         <v>1</v>
       </c>
-      <c r="B22" s="1">
-        <v>41837</v>
+      <c r="B22" s="2">
+        <v>22</v>
       </c>
       <c r="C22">
         <v>26.783333330000001</v>
@@ -7709,8 +7715,8 @@
       <c r="A23" t="b">
         <v>1</v>
       </c>
-      <c r="B23" s="1">
-        <v>41838</v>
+      <c r="B23" s="2">
+        <v>23</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -7732,8 +7738,8 @@
       <c r="A24" t="b">
         <v>0</v>
       </c>
-      <c r="B24" s="1">
-        <v>41839</v>
+      <c r="B24" s="2">
+        <v>24</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -7755,8 +7761,8 @@
       <c r="A25" t="b">
         <v>0</v>
       </c>
-      <c r="B25" s="1">
-        <v>41840</v>
+      <c r="B25" s="2">
+        <v>25</v>
       </c>
       <c r="C25">
         <v>66.900000000000006</v>
@@ -7778,8 +7784,8 @@
       <c r="A26" t="b">
         <v>0</v>
       </c>
-      <c r="B26" s="1">
-        <v>41841</v>
+      <c r="B26" s="2">
+        <v>26</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -7801,8 +7807,8 @@
       <c r="A27" t="b">
         <v>0</v>
       </c>
-      <c r="B27" s="1">
-        <v>41842</v>
+      <c r="B27" s="2">
+        <v>27</v>
       </c>
       <c r="C27">
         <v>39.683333330000004</v>
@@ -7824,8 +7830,8 @@
       <c r="A28" t="b">
         <v>0</v>
       </c>
-      <c r="B28" s="1">
-        <v>41843</v>
+      <c r="B28" s="2">
+        <v>28</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -7847,8 +7853,8 @@
       <c r="A29" t="b">
         <v>0</v>
       </c>
-      <c r="B29" s="1">
-        <v>41844</v>
+      <c r="B29" s="2">
+        <v>29</v>
       </c>
       <c r="C29">
         <v>25.65</v>
@@ -7870,8 +7876,8 @@
       <c r="A30" t="b">
         <v>0</v>
       </c>
-      <c r="B30" s="1">
-        <v>41845</v>
+      <c r="B30" s="2">
+        <v>30</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -7893,8 +7899,8 @@
       <c r="A31" t="b">
         <v>0</v>
       </c>
-      <c r="B31" s="1">
-        <v>41846</v>
+      <c r="B31" s="2">
+        <v>31</v>
       </c>
       <c r="C31">
         <v>81.566666670000004</v>
@@ -7916,8 +7922,8 @@
       <c r="A32" t="b">
         <v>0</v>
       </c>
-      <c r="B32" s="1">
-        <v>41847</v>
+      <c r="B32" s="2">
+        <v>32</v>
       </c>
       <c r="C32">
         <v>66.683333329999996</v>
@@ -7939,8 +7945,8 @@
       <c r="A33" t="b">
         <v>1</v>
       </c>
-      <c r="B33" s="1">
-        <v>41848</v>
+      <c r="B33" s="2">
+        <v>33</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -7962,8 +7968,8 @@
       <c r="A34" t="b">
         <v>1</v>
       </c>
-      <c r="B34" s="1">
-        <v>41849</v>
+      <c r="B34" s="2">
+        <v>34</v>
       </c>
       <c r="C34">
         <v>40.283333329999998</v>
@@ -7985,8 +7991,8 @@
       <c r="A35" t="b">
         <v>1</v>
       </c>
-      <c r="B35" s="1">
-        <v>41850</v>
+      <c r="B35" s="2">
+        <v>35</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -8008,8 +8014,8 @@
       <c r="A36" t="b">
         <v>1</v>
       </c>
-      <c r="B36" s="1">
-        <v>41851</v>
+      <c r="B36" s="2">
+        <v>36</v>
       </c>
       <c r="C36">
         <v>26.083333329999999</v>
@@ -8031,8 +8037,8 @@
       <c r="A37" t="b">
         <v>1</v>
       </c>
-      <c r="B37" s="1">
-        <v>41852</v>
+      <c r="B37" s="2">
+        <v>37</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -8054,8 +8060,8 @@
       <c r="A38" t="b">
         <v>1</v>
       </c>
-      <c r="B38" s="1">
-        <v>41853</v>
+      <c r="B38" s="2">
+        <v>38</v>
       </c>
       <c r="C38">
         <v>71.983333329999994</v>
@@ -8077,8 +8083,8 @@
       <c r="A39" t="b">
         <v>1</v>
       </c>
-      <c r="B39" s="1">
-        <v>41854</v>
+      <c r="B39" s="2">
+        <v>39</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -8100,8 +8106,8 @@
       <c r="A40" t="b">
         <v>1</v>
       </c>
-      <c r="B40" s="1">
-        <v>41855</v>
+      <c r="B40" s="2">
+        <v>40</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -8114,8 +8120,8 @@
       <c r="A41" t="b">
         <v>1</v>
       </c>
-      <c r="B41" s="1">
-        <v>41856</v>
+      <c r="B41" s="2">
+        <v>41</v>
       </c>
       <c r="C41">
         <v>40.633333329999999</v>
@@ -8128,8 +8134,8 @@
       <c r="A42" t="b">
         <v>1</v>
       </c>
-      <c r="B42" s="1">
-        <v>41857</v>
+      <c r="B42" s="2">
+        <v>42</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -8142,8 +8148,8 @@
       <c r="A43" t="b">
         <v>1</v>
       </c>
-      <c r="B43" s="1">
-        <v>41858</v>
+      <c r="B43" s="2">
+        <v>43</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -8156,8 +8162,8 @@
       <c r="A44" t="b">
         <v>1</v>
       </c>
-      <c r="B44" s="1">
-        <v>41859</v>
+      <c r="B44" s="2">
+        <v>44</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -8170,8 +8176,8 @@
       <c r="A45" t="b">
         <v>1</v>
       </c>
-      <c r="B45" s="1">
-        <v>41860</v>
+      <c r="B45" s="2">
+        <v>45</v>
       </c>
       <c r="C45">
         <v>0</v>
@@ -8184,8 +8190,8 @@
       <c r="A46" t="b">
         <v>1</v>
       </c>
-      <c r="B46" s="1">
-        <v>41861</v>
+      <c r="B46" s="2">
+        <v>46</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -8198,8 +8204,8 @@
       <c r="A47" t="b">
         <v>1</v>
       </c>
-      <c r="B47" s="1">
-        <v>41862</v>
+      <c r="B47" s="2">
+        <v>47</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -8212,8 +8218,8 @@
       <c r="A48" t="b">
         <v>1</v>
       </c>
-      <c r="B48" s="1">
-        <v>41863</v>
+      <c r="B48" s="2">
+        <v>48</v>
       </c>
       <c r="C48">
         <v>28.716666669999999</v>
@@ -8226,8 +8232,8 @@
       <c r="A49" t="b">
         <v>1</v>
       </c>
-      <c r="B49" s="1">
-        <v>41864</v>
+      <c r="B49" s="2">
+        <v>49</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -8240,8 +8246,8 @@
       <c r="A50" t="b">
         <v>1</v>
       </c>
-      <c r="B50" s="1">
-        <v>41865</v>
+      <c r="B50" s="2">
+        <v>50</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -8254,8 +8260,8 @@
       <c r="A51" t="b">
         <v>1</v>
       </c>
-      <c r="B51" s="1">
-        <v>41866</v>
+      <c r="B51" s="2">
+        <v>51</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -8268,8 +8274,8 @@
       <c r="A52" t="b">
         <v>1</v>
       </c>
-      <c r="B52" s="1">
-        <v>41867</v>
+      <c r="B52" s="2">
+        <v>52</v>
       </c>
       <c r="C52">
         <v>67.3</v>
@@ -8282,8 +8288,8 @@
       <c r="A53" t="b">
         <v>1</v>
       </c>
-      <c r="B53" s="1">
-        <v>41868</v>
+      <c r="B53" s="2">
+        <v>53</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -8296,8 +8302,8 @@
       <c r="A54" t="b">
         <v>1</v>
       </c>
-      <c r="B54" s="1">
-        <v>41869</v>
+      <c r="B54" s="2">
+        <v>54</v>
       </c>
       <c r="C54">
         <v>72.5</v>
@@ -8310,8 +8316,8 @@
       <c r="A55" t="b">
         <v>1</v>
       </c>
-      <c r="B55" s="1">
-        <v>41870</v>
+      <c r="B55" s="2">
+        <v>55</v>
       </c>
       <c r="C55">
         <v>60.633333329999999</v>
@@ -8324,8 +8330,8 @@
       <c r="A56" t="b">
         <v>1</v>
       </c>
-      <c r="B56" s="1">
-        <v>41871</v>
+      <c r="B56" s="2">
+        <v>56</v>
       </c>
       <c r="C56">
         <v>0</v>
@@ -8336,7 +8342,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -8344,22 +8351,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView topLeftCell="C35" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView topLeftCell="B53" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="b">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
-        <v>41810</v>
+      <c r="B1" s="2">
+        <v>1</v>
       </c>
       <c r="C1">
         <v>0</v>
@@ -8372,8 +8379,8 @@
       <c r="A2" t="b">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
-        <v>41811</v>
+      <c r="B2" s="2">
+        <v>2</v>
       </c>
       <c r="C2">
         <v>25.5</v>
@@ -8386,8 +8393,8 @@
       <c r="A3" t="b">
         <v>0</v>
       </c>
-      <c r="B3" s="1">
-        <v>41812</v>
+      <c r="B3" s="2">
+        <v>3</v>
       </c>
       <c r="C3">
         <v>39.6</v>
@@ -8400,8 +8407,8 @@
       <c r="A4" t="b">
         <v>0</v>
       </c>
-      <c r="B4" s="1">
-        <v>41813</v>
+      <c r="B4" s="2">
+        <v>4</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -8414,8 +8421,8 @@
       <c r="A5" t="b">
         <v>0</v>
       </c>
-      <c r="B5" s="1">
-        <v>41814</v>
+      <c r="B5" s="2">
+        <v>5</v>
       </c>
       <c r="C5">
         <v>66.416666669999998</v>
@@ -8428,8 +8435,8 @@
       <c r="A6" t="b">
         <v>0</v>
       </c>
-      <c r="B6" s="1">
-        <v>41815</v>
+      <c r="B6" s="2">
+        <v>6</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -8442,8 +8449,8 @@
       <c r="A7" t="b">
         <v>0</v>
       </c>
-      <c r="B7" s="1">
-        <v>41816</v>
+      <c r="B7" s="2">
+        <v>7</v>
       </c>
       <c r="C7">
         <v>80.533333330000005</v>
@@ -8456,8 +8463,8 @@
       <c r="A8" t="b">
         <v>0</v>
       </c>
-      <c r="B8" s="1">
-        <v>41817</v>
+      <c r="B8" s="2">
+        <v>8</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -8470,8 +8477,8 @@
       <c r="A9" t="b">
         <v>0</v>
       </c>
-      <c r="B9" s="1">
-        <v>41818</v>
+      <c r="B9" s="2">
+        <v>9</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -8484,8 +8491,8 @@
       <c r="A10" t="b">
         <v>0</v>
       </c>
-      <c r="B10" s="1">
-        <v>41819</v>
+      <c r="B10" s="2">
+        <v>10</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -8498,8 +8505,8 @@
       <c r="A11" t="b">
         <v>0</v>
       </c>
-      <c r="B11" s="1">
-        <v>41833</v>
+      <c r="B11" s="2">
+        <v>11</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -8512,8 +8519,8 @@
       <c r="A12" t="b">
         <v>0</v>
       </c>
-      <c r="B12" s="1">
-        <v>41834</v>
+      <c r="B12" s="2">
+        <v>12</v>
       </c>
       <c r="C12">
         <v>24.9</v>
@@ -8526,8 +8533,8 @@
       <c r="A13" t="b">
         <v>0</v>
       </c>
-      <c r="B13" s="1">
-        <v>41835</v>
+      <c r="B13" s="2">
+        <v>13</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -8540,8 +8547,8 @@
       <c r="A14" t="b">
         <v>1</v>
       </c>
-      <c r="B14" s="1">
-        <v>41836</v>
+      <c r="B14" s="2">
+        <v>14</v>
       </c>
       <c r="C14">
         <v>40.983333330000001</v>
@@ -8554,8 +8561,8 @@
       <c r="A15" t="b">
         <v>1</v>
       </c>
-      <c r="B15" s="1">
-        <v>41837</v>
+      <c r="B15" s="2">
+        <v>15</v>
       </c>
       <c r="C15">
         <v>67.433333329999996</v>
@@ -8568,8 +8575,8 @@
       <c r="A16" t="b">
         <v>1</v>
       </c>
-      <c r="B16" s="1">
-        <v>41838</v>
+      <c r="B16" s="2">
+        <v>16</v>
       </c>
       <c r="C16">
         <v>26.666666670000001</v>
@@ -8582,8 +8589,8 @@
       <c r="A17" t="b">
         <v>1</v>
       </c>
-      <c r="B17" s="1">
-        <v>41839</v>
+      <c r="B17" s="2">
+        <v>17</v>
       </c>
       <c r="C17">
         <v>81.349999999999994</v>
@@ -8596,8 +8603,8 @@
       <c r="A18" t="b">
         <v>1</v>
       </c>
-      <c r="B18" s="1">
-        <v>41840</v>
+      <c r="B18" s="2">
+        <v>18</v>
       </c>
       <c r="C18">
         <v>40.333333330000002</v>
@@ -8610,8 +8617,8 @@
       <c r="A19" t="b">
         <v>1</v>
       </c>
-      <c r="B19" s="1">
-        <v>41841</v>
+      <c r="B19" s="2">
+        <v>19</v>
       </c>
       <c r="C19">
         <v>25.8</v>
@@ -8624,8 +8631,8 @@
       <c r="A20" t="b">
         <v>1</v>
       </c>
-      <c r="B20" s="1">
-        <v>41842</v>
+      <c r="B20" s="2">
+        <v>20</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -8638,8 +8645,8 @@
       <c r="A21" t="b">
         <v>1</v>
       </c>
-      <c r="B21" s="1">
-        <v>41843</v>
+      <c r="B21" s="2">
+        <v>21</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -8652,8 +8659,8 @@
       <c r="A22" t="b">
         <v>1</v>
       </c>
-      <c r="B22" s="1">
-        <v>41844</v>
+      <c r="B22" s="2">
+        <v>22</v>
       </c>
       <c r="C22">
         <v>23.6</v>
@@ -8666,8 +8673,8 @@
       <c r="A23" t="b">
         <v>1</v>
       </c>
-      <c r="B23" s="1">
-        <v>41845</v>
+      <c r="B23" s="2">
+        <v>23</v>
       </c>
       <c r="C23">
         <v>40.25</v>
@@ -8680,8 +8687,8 @@
       <c r="A24" t="b">
         <v>1</v>
       </c>
-      <c r="B24" s="1">
-        <v>41846</v>
+      <c r="B24" s="2">
+        <v>24</v>
       </c>
       <c r="C24">
         <v>11.55</v>
@@ -8694,8 +8701,8 @@
       <c r="A25" t="b">
         <v>1</v>
       </c>
-      <c r="B25" s="1">
-        <v>41847</v>
+      <c r="B25" s="2">
+        <v>25</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -8708,8 +8715,8 @@
       <c r="A26" t="b">
         <v>1</v>
       </c>
-      <c r="B26" s="1">
-        <v>41848</v>
+      <c r="B26" s="2">
+        <v>26</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -8722,8 +8729,8 @@
       <c r="A27" t="b">
         <v>0</v>
       </c>
-      <c r="B27" s="1">
-        <v>41849</v>
+      <c r="B27" s="2">
+        <v>27</v>
       </c>
       <c r="C27">
         <v>25.35</v>
@@ -8736,8 +8743,8 @@
       <c r="A28" t="b">
         <v>0</v>
       </c>
-      <c r="B28" s="1">
-        <v>41850</v>
+      <c r="B28" s="2">
+        <v>28</v>
       </c>
       <c r="C28">
         <v>39.466666670000002</v>
@@ -8750,8 +8757,8 @@
       <c r="A29" t="b">
         <v>0</v>
       </c>
-      <c r="B29" s="1">
-        <v>41851</v>
+      <c r="B29" s="2">
+        <v>29</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -8764,8 +8771,8 @@
       <c r="A30" t="b">
         <v>0</v>
       </c>
-      <c r="B30" s="1">
-        <v>41852</v>
+      <c r="B30" s="2">
+        <v>30</v>
       </c>
       <c r="C30">
         <v>23.35</v>
@@ -8778,8 +8785,8 @@
       <c r="A31" t="b">
         <v>0</v>
       </c>
-      <c r="B31" s="1">
-        <v>41853</v>
+      <c r="B31" s="2">
+        <v>31</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -8792,8 +8799,8 @@
       <c r="A32" t="b">
         <v>0</v>
       </c>
-      <c r="B32" s="1">
-        <v>41854</v>
+      <c r="B32" s="2">
+        <v>32</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -8806,8 +8813,8 @@
       <c r="A33" t="b">
         <v>0</v>
       </c>
-      <c r="B33" s="1">
-        <v>41855</v>
+      <c r="B33" s="2">
+        <v>33</v>
       </c>
       <c r="C33">
         <v>39.466666670000002</v>
@@ -8820,8 +8827,8 @@
       <c r="A34" t="b">
         <v>0</v>
       </c>
-      <c r="B34" s="1">
-        <v>41856</v>
+      <c r="B34" s="2">
+        <v>34</v>
       </c>
       <c r="C34">
         <v>25.333333329999999</v>
@@ -8834,8 +8841,8 @@
       <c r="A35" t="b">
         <v>0</v>
       </c>
-      <c r="B35" s="1">
-        <v>41857</v>
+      <c r="B35" s="2">
+        <v>35</v>
       </c>
       <c r="C35">
         <v>66.466666669999995</v>
@@ -8848,8 +8855,8 @@
       <c r="A36" t="b">
         <v>0</v>
       </c>
-      <c r="B36" s="1">
-        <v>41858</v>
+      <c r="B36" s="2">
+        <v>36</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -8862,8 +8869,8 @@
       <c r="A37" t="b">
         <v>0</v>
       </c>
-      <c r="B37" s="1">
-        <v>41859</v>
+      <c r="B37" s="2">
+        <v>37</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -8876,8 +8883,8 @@
       <c r="A38" t="b">
         <v>0</v>
       </c>
-      <c r="B38" s="1">
-        <v>41860</v>
+      <c r="B38" s="2">
+        <v>38</v>
       </c>
       <c r="C38">
         <v>25.3</v>
@@ -8890,8 +8897,8 @@
       <c r="A39" t="b">
         <v>0</v>
       </c>
-      <c r="B39" s="1">
-        <v>41861</v>
+      <c r="B39" s="2">
+        <v>39</v>
       </c>
       <c r="C39">
         <v>39.65</v>
@@ -8904,8 +8911,8 @@
       <c r="A40" t="b">
         <v>0</v>
       </c>
-      <c r="B40" s="1">
-        <v>41862</v>
+      <c r="B40" s="2">
+        <v>40</v>
       </c>
       <c r="C40">
         <v>66.650000000000006</v>
@@ -8918,8 +8925,8 @@
       <c r="A41" t="b">
         <v>0</v>
       </c>
-      <c r="B41" s="1">
-        <v>41863</v>
+      <c r="B41" s="2">
+        <v>41</v>
       </c>
       <c r="C41">
         <v>39.683333330000004</v>
@@ -8932,8 +8939,8 @@
       <c r="A42" t="b">
         <v>0</v>
       </c>
-      <c r="B42" s="1">
-        <v>41864</v>
+      <c r="B42" s="2">
+        <v>42</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -8946,8 +8953,8 @@
       <c r="A43" t="b">
         <v>0</v>
       </c>
-      <c r="B43" s="1">
-        <v>41865</v>
+      <c r="B43" s="2">
+        <v>43</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -8960,8 +8967,8 @@
       <c r="A44" t="b">
         <v>0</v>
       </c>
-      <c r="B44" s="1">
-        <v>41866</v>
+      <c r="B44" s="2">
+        <v>44</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -8974,8 +8981,8 @@
       <c r="A45" t="b">
         <v>0</v>
       </c>
-      <c r="B45" s="1">
-        <v>41867</v>
+      <c r="B45" s="2">
+        <v>45</v>
       </c>
       <c r="C45">
         <v>82.2</v>
@@ -8988,8 +8995,8 @@
       <c r="A46" t="b">
         <v>0</v>
       </c>
-      <c r="B46" s="1">
-        <v>41868</v>
+      <c r="B46" s="2">
+        <v>46</v>
       </c>
       <c r="C46">
         <v>39.583333330000002</v>
@@ -9002,8 +9009,8 @@
       <c r="A47" t="b">
         <v>1</v>
       </c>
-      <c r="B47" s="1">
-        <v>41869</v>
+      <c r="B47" s="2">
+        <v>47</v>
       </c>
       <c r="C47">
         <v>67.366666670000001</v>
@@ -9016,8 +9023,8 @@
       <c r="A48" t="b">
         <v>1</v>
       </c>
-      <c r="B48" s="1">
-        <v>41870</v>
+      <c r="B48" s="2">
+        <v>48</v>
       </c>
       <c r="C48">
         <v>25.95</v>
@@ -9030,8 +9037,8 @@
       <c r="A49" t="b">
         <v>1</v>
       </c>
-      <c r="B49" s="1">
-        <v>41871</v>
+      <c r="B49" s="2">
+        <v>49</v>
       </c>
       <c r="C49">
         <v>67.083333330000002</v>
@@ -9044,8 +9051,8 @@
       <c r="A50" t="b">
         <v>1</v>
       </c>
-      <c r="B50" s="1">
-        <v>41872</v>
+      <c r="B50" s="2">
+        <v>50</v>
       </c>
       <c r="C50">
         <v>27.383333329999999</v>
@@ -9058,8 +9065,8 @@
       <c r="A51" t="b">
         <v>1</v>
       </c>
-      <c r="B51" s="1">
-        <v>41873</v>
+      <c r="B51" s="2">
+        <v>51</v>
       </c>
       <c r="C51">
         <v>83.933333329999996</v>
@@ -9072,8 +9079,8 @@
       <c r="A52" t="b">
         <v>1</v>
       </c>
-      <c r="B52" s="1">
-        <v>41874</v>
+      <c r="B52" s="2">
+        <v>52</v>
       </c>
       <c r="C52">
         <v>67.233333329999994</v>
@@ -9086,8 +9093,8 @@
       <c r="A53" t="b">
         <v>1</v>
       </c>
-      <c r="B53" s="1">
-        <v>41875</v>
+      <c r="B53" s="2">
+        <v>53</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -9100,8 +9107,8 @@
       <c r="A54" t="b">
         <v>1</v>
       </c>
-      <c r="B54" s="1">
-        <v>41876</v>
+      <c r="B54" s="2">
+        <v>54</v>
       </c>
       <c r="C54">
         <v>40.216666670000002</v>
@@ -9114,8 +9121,8 @@
       <c r="A55" t="b">
         <v>1</v>
       </c>
-      <c r="B55" s="1">
-        <v>41877</v>
+      <c r="B55" s="2">
+        <v>55</v>
       </c>
       <c r="C55">
         <v>21.6</v>
@@ -9128,8 +9135,8 @@
       <c r="A56" t="b">
         <v>1</v>
       </c>
-      <c r="B56" s="1">
-        <v>41878</v>
+      <c r="B56" s="2">
+        <v>56</v>
       </c>
       <c r="C56">
         <v>26.016666669999999</v>
@@ -9140,7 +9147,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -9148,21 +9156,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView topLeftCell="E34" workbookViewId="0">
-      <selection activeCell="S47" sqref="S47"/>
+    <sheetView topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="b">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
-        <v>41811</v>
+      <c r="B1" s="2">
+        <v>1</v>
       </c>
       <c r="C1">
         <v>0</v>
@@ -9175,8 +9183,8 @@
       <c r="A2" t="b">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
-        <v>41812</v>
+      <c r="B2" s="2">
+        <v>2</v>
       </c>
       <c r="C2">
         <v>26.5</v>
@@ -9189,8 +9197,8 @@
       <c r="A3" t="b">
         <v>0</v>
       </c>
-      <c r="B3" s="1">
-        <v>41813</v>
+      <c r="B3" s="2">
+        <v>3</v>
       </c>
       <c r="C3">
         <v>26.733333330000001</v>
@@ -9203,8 +9211,8 @@
       <c r="A4" t="b">
         <v>0</v>
       </c>
-      <c r="B4" s="1">
-        <v>41814</v>
+      <c r="B4" s="2">
+        <v>4</v>
       </c>
       <c r="C4">
         <v>40.866666670000001</v>
@@ -9217,8 +9225,8 @@
       <c r="A5" t="b">
         <v>0</v>
       </c>
-      <c r="B5" s="1">
-        <v>41815</v>
+      <c r="B5" s="2">
+        <v>5</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -9231,8 +9239,8 @@
       <c r="A6" t="b">
         <v>0</v>
       </c>
-      <c r="B6" s="1">
-        <v>41816</v>
+      <c r="B6" s="2">
+        <v>6</v>
       </c>
       <c r="C6">
         <v>25.2</v>
@@ -9245,8 +9253,8 @@
       <c r="A7" t="b">
         <v>0</v>
       </c>
-      <c r="B7" s="1">
-        <v>41817</v>
+      <c r="B7" s="2">
+        <v>7</v>
       </c>
       <c r="C7">
         <v>39.883333329999999</v>
@@ -9259,8 +9267,8 @@
       <c r="A8" t="b">
         <v>0</v>
       </c>
-      <c r="B8" s="1">
-        <v>41818</v>
+      <c r="B8" s="2">
+        <v>8</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -9273,8 +9281,8 @@
       <c r="A9" t="b">
         <v>0</v>
       </c>
-      <c r="B9" s="1">
-        <v>41819</v>
+      <c r="B9" s="2">
+        <v>9</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -9287,8 +9295,8 @@
       <c r="A10" t="b">
         <v>0</v>
       </c>
-      <c r="B10" s="1">
-        <v>41820</v>
+      <c r="B10" s="2">
+        <v>10</v>
       </c>
       <c r="C10">
         <v>62.35</v>
@@ -9301,8 +9309,8 @@
       <c r="A11" t="b">
         <v>0</v>
       </c>
-      <c r="B11" s="1">
-        <v>41821</v>
+      <c r="B11" s="2">
+        <v>11</v>
       </c>
       <c r="C11">
         <v>40.216666670000002</v>
@@ -9315,8 +9323,8 @@
       <c r="A12" t="b">
         <v>0</v>
       </c>
-      <c r="B12" s="1">
-        <v>41822</v>
+      <c r="B12" s="2">
+        <v>12</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -9329,8 +9337,8 @@
       <c r="A13" t="b">
         <v>1</v>
       </c>
-      <c r="B13" s="1">
-        <v>41823</v>
+      <c r="B13" s="2">
+        <v>13</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -9343,8 +9351,8 @@
       <c r="A14" t="b">
         <v>1</v>
       </c>
-      <c r="B14" s="1">
-        <v>41824</v>
+      <c r="B14" s="2">
+        <v>14</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -9357,8 +9365,8 @@
       <c r="A15" t="b">
         <v>1</v>
       </c>
-      <c r="B15" s="1">
-        <v>41825</v>
+      <c r="B15" s="2">
+        <v>15</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -9371,8 +9379,8 @@
       <c r="A16" t="b">
         <v>1</v>
       </c>
-      <c r="B16" s="1">
-        <v>41826</v>
+      <c r="B16" s="2">
+        <v>16</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -9385,8 +9393,8 @@
       <c r="A17" t="b">
         <v>1</v>
       </c>
-      <c r="B17" s="1">
-        <v>41827</v>
+      <c r="B17" s="2">
+        <v>17</v>
       </c>
       <c r="C17">
         <v>25.95</v>
@@ -9399,8 +9407,8 @@
       <c r="A18" t="b">
         <v>1</v>
       </c>
-      <c r="B18" s="1">
-        <v>41828</v>
+      <c r="B18" s="2">
+        <v>18</v>
       </c>
       <c r="C18">
         <v>25.883333329999999</v>
@@ -9413,8 +9421,8 @@
       <c r="A19" t="b">
         <v>1</v>
       </c>
-      <c r="B19" s="1">
-        <v>41829</v>
+      <c r="B19" s="2">
+        <v>19</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -9427,8 +9435,8 @@
       <c r="A20" t="b">
         <v>1</v>
       </c>
-      <c r="B20" s="1">
-        <v>41830</v>
+      <c r="B20" s="2">
+        <v>20</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -9441,8 +9449,8 @@
       <c r="A21" t="b">
         <v>1</v>
       </c>
-      <c r="B21" s="1">
-        <v>41831</v>
+      <c r="B21" s="2">
+        <v>21</v>
       </c>
       <c r="C21">
         <v>40.266666669999999</v>
@@ -9455,8 +9463,8 @@
       <c r="A22" t="b">
         <v>0</v>
       </c>
-      <c r="B22" s="1">
-        <v>41832</v>
+      <c r="B22" s="2">
+        <v>22</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -9469,8 +9477,8 @@
       <c r="A23" t="b">
         <v>0</v>
       </c>
-      <c r="B23" s="1">
-        <v>41833</v>
+      <c r="B23" s="2">
+        <v>23</v>
       </c>
       <c r="C23">
         <v>68.95</v>
@@ -9483,8 +9491,8 @@
       <c r="A24" t="b">
         <v>0</v>
       </c>
-      <c r="B24" s="1">
-        <v>41834</v>
+      <c r="B24" s="2">
+        <v>24</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -9497,8 +9505,8 @@
       <c r="A25" t="b">
         <v>0</v>
       </c>
-      <c r="B25" s="1">
-        <v>41835</v>
+      <c r="B25" s="2">
+        <v>25</v>
       </c>
       <c r="C25">
         <v>81.316666670000004</v>
@@ -9511,8 +9519,8 @@
       <c r="A26" t="b">
         <v>0</v>
       </c>
-      <c r="B26" s="1">
-        <v>41836</v>
+      <c r="B26" s="2">
+        <v>26</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -9525,8 +9533,8 @@
       <c r="A27" t="b">
         <v>0</v>
       </c>
-      <c r="B27" s="1">
-        <v>41837</v>
+      <c r="B27" s="2">
+        <v>27</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -9539,8 +9547,8 @@
       <c r="A28" t="b">
         <v>0</v>
       </c>
-      <c r="B28" s="1">
-        <v>41838</v>
+      <c r="B28" s="2">
+        <v>28</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -9553,8 +9561,8 @@
       <c r="A29" t="b">
         <v>0</v>
       </c>
-      <c r="B29" s="1">
-        <v>41839</v>
+      <c r="B29" s="2">
+        <v>29</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -9567,8 +9575,8 @@
       <c r="A30" t="b">
         <v>0</v>
       </c>
-      <c r="B30" s="1">
-        <v>41840</v>
+      <c r="B30" s="2">
+        <v>30</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -9581,8 +9589,8 @@
       <c r="A31" t="b">
         <v>0</v>
       </c>
-      <c r="B31" s="1">
-        <v>41841</v>
+      <c r="B31" s="2">
+        <v>31</v>
       </c>
       <c r="C31">
         <v>25.25</v>
@@ -9595,8 +9603,8 @@
       <c r="A32" t="b">
         <v>0</v>
       </c>
-      <c r="B32" s="1">
-        <v>41842</v>
+      <c r="B32" s="2">
+        <v>32</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -9609,8 +9617,8 @@
       <c r="A33" t="b">
         <v>0</v>
       </c>
-      <c r="B33" s="1">
-        <v>41843</v>
+      <c r="B33" s="2">
+        <v>33</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -9623,8 +9631,8 @@
       <c r="A34" t="b">
         <v>0</v>
       </c>
-      <c r="B34" s="1">
-        <v>41844</v>
+      <c r="B34" s="2">
+        <v>34</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -9637,8 +9645,8 @@
       <c r="A35" t="b">
         <v>0</v>
       </c>
-      <c r="B35" s="1">
-        <v>41845</v>
+      <c r="B35" s="2">
+        <v>35</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -9651,8 +9659,8 @@
       <c r="A36" t="b">
         <v>0</v>
       </c>
-      <c r="B36" s="1">
-        <v>41846</v>
+      <c r="B36" s="2">
+        <v>36</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -9665,8 +9673,8 @@
       <c r="A37" t="b">
         <v>0</v>
       </c>
-      <c r="B37" s="1">
-        <v>41847</v>
+      <c r="B37" s="2">
+        <v>37</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -9679,8 +9687,8 @@
       <c r="A38" t="b">
         <v>0</v>
       </c>
-      <c r="B38" s="1">
-        <v>41848</v>
+      <c r="B38" s="2">
+        <v>38</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -9693,8 +9701,8 @@
       <c r="A39" t="b">
         <v>0</v>
       </c>
-      <c r="B39" s="1">
-        <v>41849</v>
+      <c r="B39" s="2">
+        <v>39</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -9707,8 +9715,8 @@
       <c r="A40" t="b">
         <v>0</v>
       </c>
-      <c r="B40" s="1">
-        <v>41850</v>
+      <c r="B40" s="2">
+        <v>40</v>
       </c>
       <c r="C40">
         <v>25.516666669999999</v>
@@ -9721,8 +9729,8 @@
       <c r="A41" t="b">
         <v>0</v>
       </c>
-      <c r="B41" s="1">
-        <v>41851</v>
+      <c r="B41" s="2">
+        <v>41</v>
       </c>
       <c r="C41">
         <v>25.2</v>
@@ -9735,8 +9743,8 @@
       <c r="A42" t="b">
         <v>0</v>
       </c>
-      <c r="B42" s="1">
-        <v>41852</v>
+      <c r="B42" s="2">
+        <v>42</v>
       </c>
       <c r="C42">
         <v>26.1</v>
@@ -9749,8 +9757,8 @@
       <c r="A43" t="b">
         <v>0</v>
       </c>
-      <c r="B43" s="1">
-        <v>41853</v>
+      <c r="B43" s="2">
+        <v>43</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -9763,8 +9771,8 @@
       <c r="A44" t="b">
         <v>0</v>
       </c>
-      <c r="B44" s="1">
-        <v>41854</v>
+      <c r="B44" s="2">
+        <v>44</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -9777,8 +9785,8 @@
       <c r="A45" t="b">
         <v>0</v>
       </c>
-      <c r="B45" s="1">
-        <v>41855</v>
+      <c r="B45" s="2">
+        <v>45</v>
       </c>
       <c r="C45">
         <v>25.31666667</v>
@@ -9791,8 +9799,8 @@
       <c r="A46" t="b">
         <v>0</v>
       </c>
-      <c r="B46" s="1">
-        <v>41856</v>
+      <c r="B46" s="2">
+        <v>46</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -9805,8 +9813,8 @@
       <c r="A47" t="b">
         <v>0</v>
       </c>
-      <c r="B47" s="1">
-        <v>41857</v>
+      <c r="B47" s="2">
+        <v>47</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -9819,8 +9827,8 @@
       <c r="A48" t="b">
         <v>0</v>
       </c>
-      <c r="B48" s="1">
-        <v>41858</v>
+      <c r="B48" s="2">
+        <v>48</v>
       </c>
       <c r="C48">
         <v>25.18333333</v>
@@ -9833,8 +9841,8 @@
       <c r="A49" t="b">
         <v>1</v>
       </c>
-      <c r="B49" s="1">
-        <v>41859</v>
+      <c r="B49" s="2">
+        <v>49</v>
       </c>
       <c r="C49">
         <v>25.883333329999999</v>
@@ -9847,8 +9855,8 @@
       <c r="A50" t="b">
         <v>1</v>
       </c>
-      <c r="B50" s="1">
-        <v>41860</v>
+      <c r="B50" s="2">
+        <v>50</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -9861,8 +9869,8 @@
       <c r="A51" t="b">
         <v>1</v>
       </c>
-      <c r="B51" s="1">
-        <v>41861</v>
+      <c r="B51" s="2">
+        <v>51</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -9875,8 +9883,8 @@
       <c r="A52" t="b">
         <v>1</v>
       </c>
-      <c r="B52" s="1">
-        <v>41862</v>
+      <c r="B52" s="2">
+        <v>52</v>
       </c>
       <c r="C52">
         <v>26.1</v>
@@ -9889,8 +9897,8 @@
       <c r="A53" t="b">
         <v>1</v>
       </c>
-      <c r="B53" s="1">
-        <v>41863</v>
+      <c r="B53" s="2">
+        <v>53</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -9903,8 +9911,8 @@
       <c r="A54" t="b">
         <v>1</v>
       </c>
-      <c r="B54" s="1">
-        <v>41864</v>
+      <c r="B54" s="2">
+        <v>54</v>
       </c>
       <c r="C54">
         <v>25.633333329999999</v>
@@ -9917,8 +9925,8 @@
       <c r="A55" t="b">
         <v>1</v>
       </c>
-      <c r="B55" s="1">
-        <v>41865</v>
+      <c r="B55" s="2">
+        <v>55</v>
       </c>
       <c r="C55">
         <v>0</v>
@@ -9931,8 +9939,8 @@
       <c r="A56" t="b">
         <v>1</v>
       </c>
-      <c r="B56" s="1">
-        <v>41866</v>
+      <c r="B56" s="2">
+        <v>56</v>
       </c>
       <c r="C56">
         <v>0</v>
@@ -9943,7 +9951,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -9951,21 +9960,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView topLeftCell="C30" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" topLeftCell="B53" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="b">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
-        <v>41829</v>
+      <c r="B1" s="2">
+        <v>1</v>
       </c>
       <c r="C1">
         <v>0</v>
@@ -9978,8 +9987,8 @@
       <c r="A2" t="b">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
-        <v>41830</v>
+      <c r="B2" s="2">
+        <v>2</v>
       </c>
       <c r="C2">
         <v>21.633333329999999</v>
@@ -9992,8 +10001,8 @@
       <c r="A3" t="b">
         <v>0</v>
       </c>
-      <c r="B3" s="1">
-        <v>41831</v>
+      <c r="B3" s="2">
+        <v>3</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -10006,8 +10015,8 @@
       <c r="A4" t="b">
         <v>0</v>
       </c>
-      <c r="B4" s="1">
-        <v>41832</v>
+      <c r="B4" s="2">
+        <v>4</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -10020,8 +10029,8 @@
       <c r="A5" t="b">
         <v>0</v>
       </c>
-      <c r="B5" s="1">
-        <v>41833</v>
+      <c r="B5" s="2">
+        <v>5</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -10034,8 +10043,8 @@
       <c r="A6" t="b">
         <v>0</v>
       </c>
-      <c r="B6" s="1">
-        <v>41834</v>
+      <c r="B6" s="2">
+        <v>6</v>
       </c>
       <c r="C6">
         <v>24.366666670000001</v>
@@ -10048,8 +10057,8 @@
       <c r="A7" t="b">
         <v>0</v>
       </c>
-      <c r="B7" s="1">
-        <v>41835</v>
+      <c r="B7" s="2">
+        <v>7</v>
       </c>
       <c r="C7">
         <v>39.833333330000002</v>
@@ -10062,8 +10071,8 @@
       <c r="A8" t="b">
         <v>0</v>
       </c>
-      <c r="B8" s="1">
-        <v>41836</v>
+      <c r="B8" s="2">
+        <v>8</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -10076,8 +10085,8 @@
       <c r="A9" t="b">
         <v>0</v>
       </c>
-      <c r="B9" s="1">
-        <v>41837</v>
+      <c r="B9" s="2">
+        <v>9</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -10090,8 +10099,8 @@
       <c r="A10" t="b">
         <v>0</v>
       </c>
-      <c r="B10" s="1">
-        <v>41838</v>
+      <c r="B10" s="2">
+        <v>10</v>
       </c>
       <c r="C10">
         <v>25.116666670000001</v>
@@ -10104,8 +10113,8 @@
       <c r="A11" t="b">
         <v>0</v>
       </c>
-      <c r="B11" s="1">
-        <v>41839</v>
+      <c r="B11" s="2">
+        <v>11</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -10118,8 +10127,8 @@
       <c r="A12" t="b">
         <v>0</v>
       </c>
-      <c r="B12" s="1">
-        <v>41840</v>
+      <c r="B12" s="2">
+        <v>12</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -10132,8 +10141,8 @@
       <c r="A13" t="b">
         <v>0</v>
       </c>
-      <c r="B13" s="1">
-        <v>41841</v>
+      <c r="B13" s="2">
+        <v>13</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -10146,8 +10155,8 @@
       <c r="A14" t="b">
         <v>0</v>
       </c>
-      <c r="B14" s="1">
-        <v>41842</v>
+      <c r="B14" s="2">
+        <v>14</v>
       </c>
       <c r="C14">
         <v>14.383333329999999</v>
@@ -10160,8 +10169,8 @@
       <c r="A15" t="b">
         <v>0</v>
       </c>
-      <c r="B15" s="1">
-        <v>41843</v>
+      <c r="B15" s="2">
+        <v>15</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -10174,8 +10183,8 @@
       <c r="A16" t="b">
         <v>0</v>
       </c>
-      <c r="B16" s="1">
-        <v>41844</v>
+      <c r="B16" s="2">
+        <v>16</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -10188,8 +10197,8 @@
       <c r="A17" t="b">
         <v>0</v>
       </c>
-      <c r="B17" s="1">
-        <v>41845</v>
+      <c r="B17" s="2">
+        <v>17</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -10202,8 +10211,8 @@
       <c r="A18" t="b">
         <v>0</v>
       </c>
-      <c r="B18" s="1">
-        <v>41846</v>
+      <c r="B18" s="2">
+        <v>18</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -10216,8 +10225,8 @@
       <c r="A19" t="b">
         <v>0</v>
       </c>
-      <c r="B19" s="1">
-        <v>41847</v>
+      <c r="B19" s="2">
+        <v>19</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -10230,8 +10239,8 @@
       <c r="A20" t="b">
         <v>1</v>
       </c>
-      <c r="B20" s="1">
-        <v>41848</v>
+      <c r="B20" s="2">
+        <v>20</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -10244,8 +10253,8 @@
       <c r="A21" t="b">
         <v>1</v>
       </c>
-      <c r="B21" s="1">
-        <v>41849</v>
+      <c r="B21" s="2">
+        <v>21</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -10258,8 +10267,8 @@
       <c r="A22" t="b">
         <v>1</v>
       </c>
-      <c r="B22" s="1">
-        <v>41850</v>
+      <c r="B22" s="2">
+        <v>22</v>
       </c>
       <c r="C22">
         <v>25.483333330000001</v>
@@ -10272,8 +10281,8 @@
       <c r="A23" t="b">
         <v>1</v>
       </c>
-      <c r="B23" s="1">
-        <v>41851</v>
+      <c r="B23" s="2">
+        <v>23</v>
       </c>
       <c r="C23">
         <v>72.666666669999998</v>
@@ -10286,8 +10295,8 @@
       <c r="A24" t="b">
         <v>1</v>
       </c>
-      <c r="B24" s="1">
-        <v>41852</v>
+      <c r="B24" s="2">
+        <v>24</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -10300,8 +10309,8 @@
       <c r="A25" t="b">
         <v>1</v>
       </c>
-      <c r="B25" s="1">
-        <v>41853</v>
+      <c r="B25" s="2">
+        <v>25</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -10314,8 +10323,8 @@
       <c r="A26" t="b">
         <v>1</v>
       </c>
-      <c r="B26" s="1">
-        <v>41854</v>
+      <c r="B26" s="2">
+        <v>26</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -10328,8 +10337,8 @@
       <c r="A27" t="b">
         <v>1</v>
       </c>
-      <c r="B27" s="1">
-        <v>41855</v>
+      <c r="B27" s="2">
+        <v>27</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -10342,8 +10351,8 @@
       <c r="A28" t="b">
         <v>1</v>
       </c>
-      <c r="B28" s="1">
-        <v>41856</v>
+      <c r="B28" s="2">
+        <v>28</v>
       </c>
       <c r="C28">
         <v>30.55</v>
@@ -10356,8 +10365,8 @@
       <c r="A29" t="b">
         <v>1</v>
       </c>
-      <c r="B29" s="1">
-        <v>41857</v>
+      <c r="B29" s="2">
+        <v>29</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -10370,8 +10379,8 @@
       <c r="A30" t="b">
         <v>1</v>
       </c>
-      <c r="B30" s="1">
-        <v>41858</v>
+      <c r="B30" s="2">
+        <v>30</v>
       </c>
       <c r="C30">
         <v>75.766666670000006</v>
@@ -10384,8 +10393,8 @@
       <c r="A31" t="b">
         <v>1</v>
       </c>
-      <c r="B31" s="1">
-        <v>41859</v>
+      <c r="B31" s="2">
+        <v>31</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -10398,8 +10407,8 @@
       <c r="A32" t="b">
         <v>0</v>
       </c>
-      <c r="B32" s="1">
-        <v>41860</v>
+      <c r="B32" s="2">
+        <v>32</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -10412,8 +10421,8 @@
       <c r="A33" t="b">
         <v>0</v>
       </c>
-      <c r="B33" s="1">
-        <v>41861</v>
+      <c r="B33" s="2">
+        <v>33</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -10426,8 +10435,8 @@
       <c r="A34" t="b">
         <v>0</v>
       </c>
-      <c r="B34" s="1">
-        <v>41862</v>
+      <c r="B34" s="2">
+        <v>34</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -10440,8 +10449,8 @@
       <c r="A35" t="b">
         <v>0</v>
       </c>
-      <c r="B35" s="1">
-        <v>41863</v>
+      <c r="B35" s="2">
+        <v>35</v>
       </c>
       <c r="C35">
         <v>29.283333330000001</v>
@@ -10454,8 +10463,8 @@
       <c r="A36" t="b">
         <v>0</v>
       </c>
-      <c r="B36" s="1">
-        <v>41864</v>
+      <c r="B36" s="2">
+        <v>36</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -10468,8 +10477,8 @@
       <c r="A37" t="b">
         <v>0</v>
       </c>
-      <c r="B37" s="1">
-        <v>41865</v>
+      <c r="B37" s="2">
+        <v>37</v>
       </c>
       <c r="C37">
         <v>25.1</v>
@@ -10482,8 +10491,8 @@
       <c r="A38" t="b">
         <v>0</v>
       </c>
-      <c r="B38" s="1">
-        <v>41866</v>
+      <c r="B38" s="2">
+        <v>38</v>
       </c>
       <c r="C38">
         <v>25.233333330000001</v>
@@ -10496,8 +10505,8 @@
       <c r="A39" t="b">
         <v>0</v>
       </c>
-      <c r="B39" s="1">
-        <v>41867</v>
+      <c r="B39" s="2">
+        <v>39</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -10510,8 +10519,8 @@
       <c r="A40" t="b">
         <v>0</v>
       </c>
-      <c r="B40" s="1">
-        <v>41868</v>
+      <c r="B40" s="2">
+        <v>40</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -10524,8 +10533,8 @@
       <c r="A41" t="b">
         <v>1</v>
       </c>
-      <c r="B41" s="1">
-        <v>41869</v>
+      <c r="B41" s="2">
+        <v>41</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -10538,8 +10547,8 @@
       <c r="A42" t="b">
         <v>1</v>
       </c>
-      <c r="B42" s="1">
-        <v>41870</v>
+      <c r="B42" s="2">
+        <v>42</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -10552,8 +10561,8 @@
       <c r="A43" t="b">
         <v>1</v>
       </c>
-      <c r="B43" s="1">
-        <v>41871</v>
+      <c r="B43" s="2">
+        <v>43</v>
       </c>
       <c r="C43">
         <v>25.883333329999999</v>
@@ -10566,8 +10575,8 @@
       <c r="A44" t="b">
         <v>1</v>
       </c>
-      <c r="B44" s="1">
-        <v>41872</v>
+      <c r="B44" s="2">
+        <v>44</v>
       </c>
       <c r="C44">
         <v>8</v>
@@ -10580,8 +10589,8 @@
       <c r="A45" t="b">
         <v>1</v>
       </c>
-      <c r="B45" s="1">
-        <v>41873</v>
+      <c r="B45" s="2">
+        <v>45</v>
       </c>
       <c r="C45">
         <v>0</v>
@@ -10594,8 +10603,8 @@
       <c r="A46" t="b">
         <v>1</v>
       </c>
-      <c r="B46" s="1">
-        <v>41874</v>
+      <c r="B46" s="2">
+        <v>46</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -10608,8 +10617,8 @@
       <c r="A47" t="b">
         <v>1</v>
       </c>
-      <c r="B47" s="1">
-        <v>41875</v>
+      <c r="B47" s="2">
+        <v>47</v>
       </c>
       <c r="C47">
         <v>26.383333329999999</v>
@@ -10622,8 +10631,8 @@
       <c r="A48" t="b">
         <v>1</v>
       </c>
-      <c r="B48" s="1">
-        <v>41876</v>
+      <c r="B48" s="2">
+        <v>48</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -10636,8 +10645,8 @@
       <c r="A49" t="b">
         <v>1</v>
       </c>
-      <c r="B49" s="1">
-        <v>41877</v>
+      <c r="B49" s="2">
+        <v>49</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -10650,8 +10659,8 @@
       <c r="A50" t="b">
         <v>1</v>
       </c>
-      <c r="B50" s="1">
-        <v>41878</v>
+      <c r="B50" s="2">
+        <v>50</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -10664,8 +10673,8 @@
       <c r="A51" t="b">
         <v>1</v>
       </c>
-      <c r="B51" s="1">
-        <v>41879</v>
+      <c r="B51" s="2">
+        <v>51</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -10678,8 +10687,8 @@
       <c r="A52" t="b">
         <v>1</v>
       </c>
-      <c r="B52" s="1">
-        <v>41880</v>
+      <c r="B52" s="2">
+        <v>52</v>
       </c>
       <c r="C52">
         <v>7.3333333329999997</v>
@@ -10692,8 +10701,8 @@
       <c r="A53" t="b">
         <v>1</v>
       </c>
-      <c r="B53" s="1">
-        <v>41881</v>
+      <c r="B53" s="2">
+        <v>53</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -10706,8 +10715,8 @@
       <c r="A54" t="b">
         <v>1</v>
       </c>
-      <c r="B54" s="1">
-        <v>41882</v>
+      <c r="B54" s="2">
+        <v>54</v>
       </c>
       <c r="C54">
         <v>25.68333333</v>
@@ -10720,8 +10729,8 @@
       <c r="A55" t="b">
         <v>1</v>
       </c>
-      <c r="B55" s="1">
-        <v>41883</v>
+      <c r="B55" s="2">
+        <v>55</v>
       </c>
       <c r="C55">
         <v>0</v>
@@ -10734,8 +10743,8 @@
       <c r="A56" t="b">
         <v>1</v>
       </c>
-      <c r="B56" s="1">
-        <v>41884</v>
+      <c r="B56" s="2">
+        <v>56</v>
       </c>
       <c r="C56">
         <v>24.783333330000001</v>
@@ -10746,6 +10755,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>